<commit_message>
Refactor code to filter data by target gene and sample name
</commit_message>
<xml_diff>
--- a/TN042/ddct_dox.xlsx
+++ b/TN042/ddct_dox.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="B1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,20 +450,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.5864994333333335</v>
-      </c>
-      <c r="C2" t="n">
-        <v>-1.147916233333333</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.2273942333333316</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update target gene names in TN042.3.py
</commit_message>
<xml_diff>
--- a/TN042/ddct_dox.xlsx
+++ b/TN042/ddct_dox.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,20 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5864994333333335</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-1.147916233333333</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.2273942333333316</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add altair library and generate plots for fold change
</commit_message>
<xml_diff>
--- a/TN042/ddct_dox.xlsx
+++ b/TN042/ddct_dox.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,17 +436,12 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>dusp11</t>
+          <t>Condition</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>ifnb</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>mx1</t>
+          <t>ddCT</t>
         </is>
       </c>
     </row>
@@ -454,13 +449,38 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dusp11</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>0.5864994333333335</v>
       </c>
-      <c r="C2" t="n">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ifnb</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>-1.147916233333333</v>
       </c>
-      <c r="D2" t="n">
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mx1</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>-0.2273942333333316</v>
       </c>
     </row>

</xml_diff>